<commit_message>
Yes, now knipex is done!
</commit_message>
<xml_diff>
--- a/knipex.xlsx
+++ b/knipex.xlsx
@@ -872,7 +872,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>4003773022992</t>
+          <t>4003773034094</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -882,14 +882,14 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://www.knipex.com/fileadmin/site/knipex/scripts/mediando/images/KNIPEX/Produktfotos/web/zoom/8801250-02-1.jpg</t>
+          <t>https://www.knipex.com/fileadmin/site/knipex/scripts/mediando/images/KNIPEX/Produktfotos/web/zoom/8801300-01-1.jpg</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>4003773034094</t>
+          <t>4003773022992</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://www.knipex.com/fileadmin/site/knipex/scripts/mediando/images/KNIPEX/Produktfotos/web/zoom/8801300-01-1.jpg</t>
+          <t>https://www.knipex.com/fileadmin/site/knipex/scripts/mediando/images/KNIPEX/Produktfotos/web/zoom/8801250-02-1.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>